<commit_message>
Cleaning flaskIO code, deleting extra non-related lines.
</commit_message>
<xml_diff>
--- a/businessNeed.xlsx
+++ b/businessNeed.xlsx
@@ -10,7 +10,7 @@
     <sheet name="owssvr" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr" localSheetId="0" hidden="1">owssvr!$A$1:$F$16</definedName>
+    <definedName name="owssvr" localSheetId="0" hidden="1">owssvr!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -18,14 +18,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\bfarhoudi\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.IE5\TXQF9HDM\owssvr.iqy" keepAlive="1" name="owssvr" type="5" refreshedVersion="4" minRefreshableVersion="3" saveData="1">
+  <connection id="1" odcFile="C:\Users\bfarhoudi\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.IE5\0Q9KCA66\owssvr.iqy" keepAlive="1" name="owssvr" type="5" refreshedVersion="4" minRefreshableVersion="3" saveData="1">
     <dbPr connection="Provider=Microsoft.Office.List.OLEDB.2.0;Data Source=&quot;&quot;;ApplicationName=Excel;Version=12.0.0.0" command="&lt;LIST&gt;&lt;VIEWGUID&gt;{A3F584F5-F858-4025-8B0B-4DDE7EA26028}&lt;/VIEWGUID&gt;&lt;LISTNAME&gt;{9DC112D0-A174-4C6E-93A2-C46287E0530E}&lt;/LISTNAME&gt;&lt;LISTWEB&gt;https://share.ahsnet.ca/teams/kmqa/_vti_bin&lt;/LISTWEB&gt;&lt;LISTSUBWEB&gt;&lt;/LISTSUBWEB&gt;&lt;ROOTFOLDER&gt;/teams/kmqa/Lists/Business Need&lt;/ROOTFOLDER&gt;&lt;/LIST&gt;" commandType="5"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Business Need</t>
   </si>
@@ -60,6 +60,15 @@
     <t>Item</t>
   </si>
   <si>
+    <t>Audio Recording</t>
+  </si>
+  <si>
+    <t>_Starting Over;#24;#Adobe Audition;#54</t>
+  </si>
+  <si>
+    <t>_Starting Over;#22;#Audio;#61</t>
+  </si>
+  <si>
     <t>Brainstorming</t>
   </si>
   <si>
@@ -87,7 +96,7 @@
     <t>Communication</t>
   </si>
   <si>
-    <t>_Starting Over;#22;#InfoGraphic;#47;#Posters;#48;#New Letters;#49;#Memes and Vemes;#50</t>
+    <t>_Starting Over;#22;#InfoGraphic;#47;#Posters;#48;#Newsletter;#49;#Memes and Vemes;#50</t>
   </si>
   <si>
     <t>Posters</t>
@@ -132,10 +141,10 @@
     <t>Learning</t>
   </si>
   <si>
-    <t>_Starting Over;#24;#Adobe Acrobat 9 Pro;#34;#Adobe eLearning;#35;#Presenter Media;#36;#Prezi;#37;#Prespectore;#38;#Microsoft PowerPoint;#39;#Microsoft Word;#50</t>
-  </si>
-  <si>
-    <t>_Starting Over;#22;#Curriculum;#34;#eBook;#35;#Job Aid;#36;#Online Module;#37;#Presentations;#38;#Training Manual;#39</t>
+    <t>_Starting Over;#24;#Adobe Acrobat Pro;#34;#Adobe eLearning;#35;#Presenter Media;#36;#Prezi;#37;#Prespectore;#38;#Microsoft PowerPoint;#39;#Microsoft Word;#50;#Adobe Lifecycle;#51;#Designer ES2;#52;#Microsoft Publisher;#53</t>
+  </si>
+  <si>
+    <t>_Starting Over;#22;#Curriculum;#34;#eBook;#35;#Job Aid;#36;#Online Module;#37;#Presentations;#38;#Training Manual;#39;#Information Sheet;#60</t>
   </si>
   <si>
     <t>Referencing</t>
@@ -153,7 +162,7 @@
     <t>_Starting Over;#24;#SharePoint;#29;#nVivo;#42;#KRS Lib Guides;#43</t>
   </si>
   <si>
-    <t>_Starting Over;#22;#Qualitative and Quantitative Analysis;#42;#Knowledge Repositories;#43;#Literature Review;#44</t>
+    <t>_Starting Over;#22;#Qualitative and Quantitative Analysis;#42;#Knowledge Repositories;#43;#Literature Review;#44;#Environmental Scan;#59;#Literature Search;#62;#Systematic Review;#63;#Evidence Summary;#64</t>
   </si>
   <si>
     <t>Simulation</t>
@@ -171,7 +180,7 @@
     <t>Videography</t>
   </si>
   <si>
-    <t>_Starting Over;#24;#Soney Vegas;#47</t>
+    <t>_Starting Over;#24;#Soney Vegas;#47;#Go Animate;#55</t>
   </si>
   <si>
     <t>_Starting Over;#22;#Video;#45</t>
@@ -750,8 +759,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr" displayName="Table_owssvr" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr" displayName="Table_owssvr" ref="A1:F17" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
     <tableColumn id="1" uniqueName="Title" name="Business Need" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" uniqueName="Related_x005f_x0020_Software" name="Related Software" queryTableFieldId="2"/>
@@ -1051,7 +1060,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1112,9 +1121,7 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1124,16 +1131,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -1144,10 +1151,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1167,12 +1174,14 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1203,10 +1212,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -1218,13 +1227,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -1236,13 +1245,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -1329,10 +1338,10 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1344,19 +1353,37 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>